<commit_message>
Add pyomo model and add parameter data in the dados.xlsx sheet
</commit_message>
<xml_diff>
--- a/dados/dados.xlsx
+++ b/dados/dados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\je4hu\colrepos\otimizacao\trabalho_final\dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7620E78B-0154-4A67-A8FD-5752630893FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5102E94D-E7AD-4D0D-AB7F-C51EA0F20974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{0ED698B2-3675-430C-AEB8-BE1A45408D0F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="746" firstSheet="2" activeTab="5" xr2:uid="{0ED698B2-3675-430C-AEB8-BE1A45408D0F}"/>
   </bookViews>
   <sheets>
     <sheet name="custo_energia" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="producao_maxima" sheetId="3" r:id="rId3"/>
     <sheet name="demanda_minima" sheetId="4" r:id="rId4"/>
     <sheet name="distribuicao_maxima" sheetId="5" r:id="rId5"/>
+    <sheet name="demanda_municipios" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="49">
   <si>
     <t>Sistema Alto do Céu</t>
   </si>
@@ -1436,7 +1437,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1565,12 +1566,13 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A2" sqref="A2:A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -1679,6 +1681,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1686,8 +1689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{150CFC59-9CFD-4E7B-BFB5-6646BB23A893}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2036,4 +2039,473 @@
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDBCD47A-28C8-46BE-9EE8-29D875476318}">
+  <dimension ref="A1:M11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="1">
+        <v>41275</v>
+      </c>
+      <c r="C1" s="1">
+        <v>41306</v>
+      </c>
+      <c r="D1" s="1">
+        <v>41334</v>
+      </c>
+      <c r="E1" s="1">
+        <v>41365</v>
+      </c>
+      <c r="F1" s="1">
+        <v>41395</v>
+      </c>
+      <c r="G1" s="1">
+        <v>41426</v>
+      </c>
+      <c r="H1" s="1">
+        <v>41456</v>
+      </c>
+      <c r="I1" s="1">
+        <v>41487</v>
+      </c>
+      <c r="J1" s="1">
+        <v>41518</v>
+      </c>
+      <c r="K1" s="1">
+        <v>41548</v>
+      </c>
+      <c r="L1" s="1">
+        <v>41579</v>
+      </c>
+      <c r="M1" s="1">
+        <v>41609</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2">
+        <v>14400000</v>
+      </c>
+      <c r="C2">
+        <v>11800000</v>
+      </c>
+      <c r="D2">
+        <v>10800000</v>
+      </c>
+      <c r="E2">
+        <v>10800000</v>
+      </c>
+      <c r="F2">
+        <v>12100000</v>
+      </c>
+      <c r="G2">
+        <v>12800000</v>
+      </c>
+      <c r="H2">
+        <v>13100000</v>
+      </c>
+      <c r="I2">
+        <v>12900000</v>
+      </c>
+      <c r="J2">
+        <v>13000000</v>
+      </c>
+      <c r="K2">
+        <v>13800000</v>
+      </c>
+      <c r="L2">
+        <v>12300000</v>
+      </c>
+      <c r="M2">
+        <v>12200000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3">
+        <v>3600000</v>
+      </c>
+      <c r="C3">
+        <v>2500000</v>
+      </c>
+      <c r="D3">
+        <v>4700000</v>
+      </c>
+      <c r="E3">
+        <v>4200000</v>
+      </c>
+      <c r="F3">
+        <v>4100000</v>
+      </c>
+      <c r="G3">
+        <v>3700000</v>
+      </c>
+      <c r="H3">
+        <v>3800000</v>
+      </c>
+      <c r="I3">
+        <v>4300000</v>
+      </c>
+      <c r="J3">
+        <v>3800000</v>
+      </c>
+      <c r="K3">
+        <v>4800000</v>
+      </c>
+      <c r="L3">
+        <v>4500000</v>
+      </c>
+      <c r="M3">
+        <v>4400000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4">
+        <v>1800000</v>
+      </c>
+      <c r="C4">
+        <v>1500000</v>
+      </c>
+      <c r="D4">
+        <v>3000000</v>
+      </c>
+      <c r="E4">
+        <v>2600000</v>
+      </c>
+      <c r="F4">
+        <v>2500000</v>
+      </c>
+      <c r="G4">
+        <v>2900000</v>
+      </c>
+      <c r="H4">
+        <v>2800000</v>
+      </c>
+      <c r="I4">
+        <v>3000000</v>
+      </c>
+      <c r="J4">
+        <v>2700000</v>
+      </c>
+      <c r="K4">
+        <v>2900000</v>
+      </c>
+      <c r="L4">
+        <v>2400000</v>
+      </c>
+      <c r="M4">
+        <v>2500000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5">
+        <v>1500000</v>
+      </c>
+      <c r="C5">
+        <v>1400000</v>
+      </c>
+      <c r="D5">
+        <v>1500000</v>
+      </c>
+      <c r="E5">
+        <v>1400000</v>
+      </c>
+      <c r="F5">
+        <v>1400000</v>
+      </c>
+      <c r="G5">
+        <v>1400000</v>
+      </c>
+      <c r="H5">
+        <v>1700000</v>
+      </c>
+      <c r="I5">
+        <v>1600000</v>
+      </c>
+      <c r="J5">
+        <v>1300000</v>
+      </c>
+      <c r="K5">
+        <v>1400000</v>
+      </c>
+      <c r="L5">
+        <v>1500000</v>
+      </c>
+      <c r="M5">
+        <v>1900000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6">
+        <v>1300000</v>
+      </c>
+      <c r="C6">
+        <v>1400000</v>
+      </c>
+      <c r="D6">
+        <v>1200000</v>
+      </c>
+      <c r="E6">
+        <v>1100000</v>
+      </c>
+      <c r="F6">
+        <v>1400000</v>
+      </c>
+      <c r="G6">
+        <v>1300000</v>
+      </c>
+      <c r="H6">
+        <v>1500000</v>
+      </c>
+      <c r="I6">
+        <v>1700000</v>
+      </c>
+      <c r="J6">
+        <v>1300000</v>
+      </c>
+      <c r="K6">
+        <v>1500000</v>
+      </c>
+      <c r="L6">
+        <v>1100000</v>
+      </c>
+      <c r="M6">
+        <v>1100000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7">
+        <v>1200000</v>
+      </c>
+      <c r="C7">
+        <v>1200000</v>
+      </c>
+      <c r="D7">
+        <v>1300000</v>
+      </c>
+      <c r="E7">
+        <v>1100000</v>
+      </c>
+      <c r="F7">
+        <v>1200000</v>
+      </c>
+      <c r="G7">
+        <v>1200000</v>
+      </c>
+      <c r="H7">
+        <v>800000</v>
+      </c>
+      <c r="I7">
+        <v>1100000</v>
+      </c>
+      <c r="J7">
+        <v>1000000</v>
+      </c>
+      <c r="K7">
+        <v>1000000</v>
+      </c>
+      <c r="L7">
+        <v>1100000</v>
+      </c>
+      <c r="M7">
+        <v>1100000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8">
+        <v>700000</v>
+      </c>
+      <c r="C8">
+        <v>500000</v>
+      </c>
+      <c r="D8">
+        <v>350000</v>
+      </c>
+      <c r="E8">
+        <v>450000</v>
+      </c>
+      <c r="F8">
+        <v>500000</v>
+      </c>
+      <c r="G8">
+        <v>500000</v>
+      </c>
+      <c r="H8">
+        <v>750000</v>
+      </c>
+      <c r="I8">
+        <v>750000</v>
+      </c>
+      <c r="J8">
+        <v>750000</v>
+      </c>
+      <c r="K8">
+        <v>750000</v>
+      </c>
+      <c r="L8">
+        <v>750000</v>
+      </c>
+      <c r="M8">
+        <v>750000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9">
+        <v>300000</v>
+      </c>
+      <c r="C9">
+        <v>200000</v>
+      </c>
+      <c r="D9">
+        <v>300000</v>
+      </c>
+      <c r="E9">
+        <v>300000</v>
+      </c>
+      <c r="F9">
+        <v>200000</v>
+      </c>
+      <c r="G9">
+        <v>300000</v>
+      </c>
+      <c r="H9">
+        <v>300000</v>
+      </c>
+      <c r="I9">
+        <v>250000</v>
+      </c>
+      <c r="J9">
+        <v>500000</v>
+      </c>
+      <c r="K9">
+        <v>350000</v>
+      </c>
+      <c r="L9">
+        <v>350000</v>
+      </c>
+      <c r="M9">
+        <v>450000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10">
+        <v>200000</v>
+      </c>
+      <c r="C10">
+        <v>180000</v>
+      </c>
+      <c r="D10">
+        <v>200000</v>
+      </c>
+      <c r="E10">
+        <v>200000</v>
+      </c>
+      <c r="F10">
+        <v>210000</v>
+      </c>
+      <c r="G10">
+        <v>210000</v>
+      </c>
+      <c r="H10">
+        <v>240000</v>
+      </c>
+      <c r="I10">
+        <v>270000</v>
+      </c>
+      <c r="J10">
+        <v>260000</v>
+      </c>
+      <c r="K10">
+        <v>270000</v>
+      </c>
+      <c r="L10">
+        <v>280000</v>
+      </c>
+      <c r="M10">
+        <v>240000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11">
+        <v>130000</v>
+      </c>
+      <c r="C11">
+        <v>110000</v>
+      </c>
+      <c r="D11">
+        <v>170000</v>
+      </c>
+      <c r="E11">
+        <v>160000</v>
+      </c>
+      <c r="F11">
+        <v>170000</v>
+      </c>
+      <c r="G11">
+        <v>160000</v>
+      </c>
+      <c r="H11">
+        <v>170000</v>
+      </c>
+      <c r="I11">
+        <v>170000</v>
+      </c>
+      <c r="J11">
+        <v>160000</v>
+      </c>
+      <c r="K11">
+        <v>170000</v>
+      </c>
+      <c r="L11">
+        <v>160000</v>
+      </c>
+      <c r="M11">
+        <v>110000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>